<commit_message>
add noviat 70 modules
</commit_message>
<xml_diff>
--- a/account_move_import/sample_import_file/account_move_lines.xlsx
+++ b/account_move_import/sample_import_file/account_move_lines.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr date1904="1" defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OpenERP\@SVN\Noviat_Generic\V8.0\account_move_import\sample_import_file\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="315" yWindow="345" windowWidth="25710" windowHeight="8850" tabRatio="489"/>
   </bookViews>
@@ -17,7 +12,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'OE Suppliers EUR'!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -42,6 +37,15 @@
     <t>account</t>
   </si>
   <si>
+    <t>OpenERP</t>
+  </si>
+  <si>
+    <t>PI12/0101</t>
+  </si>
+  <si>
+    <t>PI12/0250</t>
+  </si>
+  <si>
     <t>032/0029</t>
   </si>
   <si>
@@ -54,19 +58,10 @@
     <t>Balance suppliers Opening Entry</t>
   </si>
   <si>
-    <t>ASUSTeK</t>
-  </si>
-  <si>
-    <t>Open Invoice from supplier ASUSTeK</t>
-  </si>
-  <si>
-    <t>PI14/0250</t>
-  </si>
-  <si>
-    <t>PI14/0101</t>
-  </si>
-  <si>
-    <t>Open Invoice from supplier with reference '032/0029'</t>
+    <t>Open Invoice from supplier OpenERP</t>
+  </si>
+  <si>
+    <t>Open Invoice from customer with reference '032/0029'</t>
   </si>
 </sst>
 </file>
@@ -251,9 +246,6 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -301,7 +293,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -336,7 +328,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -554,7 +546,7 @@
       <pane xSplit="6" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E8" sqref="E8"/>
+      <selection pane="bottomRight" activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -590,12 +582,12 @@
       </c>
       <c r="G1" s="13"/>
       <c r="H1" s="2" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C2" s="7">
         <v>440000</v>
@@ -609,21 +601,21 @@
       </c>
       <c r="G2" s="14"/>
       <c r="H2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C3" s="7">
         <v>440000</v>
       </c>
       <c r="D3" s="9">
-        <v>40554</v>
+        <v>39824</v>
       </c>
       <c r="E3" s="11">
         <v>0</v>
@@ -633,21 +625,21 @@
       </c>
       <c r="G3" s="14"/>
       <c r="H3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C4" s="7">
         <v>440000</v>
       </c>
       <c r="D4" s="9">
-        <v>40574</v>
+        <v>39844</v>
       </c>
       <c r="E4" s="11">
         <v>0</v>

</xml_diff>

<commit_message>
add noviat 6.1 modules
</commit_message>
<xml_diff>
--- a/account_move_import/sample_import_file/account_move_lines.xlsx
+++ b/account_move_import/sample_import_file/account_move_lines.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr date1904="1" defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OpenERP\@SVN\Noviat_Generic\V8.0\account_move_import\sample_import_file\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="315" yWindow="345" windowWidth="25710" windowHeight="8850" tabRatio="489"/>
   </bookViews>
@@ -17,7 +12,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'OE Suppliers EUR'!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -42,6 +37,15 @@
     <t>account</t>
   </si>
   <si>
+    <t>OpenERP</t>
+  </si>
+  <si>
+    <t>PI12/0101</t>
+  </si>
+  <si>
+    <t>PI12/0250</t>
+  </si>
+  <si>
     <t>032/0029</t>
   </si>
   <si>
@@ -54,19 +58,10 @@
     <t>Balance suppliers Opening Entry</t>
   </si>
   <si>
-    <t>ASUSTeK</t>
-  </si>
-  <si>
-    <t>Open Invoice from supplier ASUSTeK</t>
-  </si>
-  <si>
-    <t>PI14/0250</t>
-  </si>
-  <si>
-    <t>PI14/0101</t>
-  </si>
-  <si>
-    <t>Open Invoice from supplier with reference '032/0029'</t>
+    <t>Open Invoice from supplier OpenERP</t>
+  </si>
+  <si>
+    <t>Open Invoice from customer with reference '032/0029'</t>
   </si>
 </sst>
 </file>
@@ -251,9 +246,6 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -301,7 +293,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -336,7 +328,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -554,7 +546,7 @@
       <pane xSplit="6" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E8" sqref="E8"/>
+      <selection pane="bottomRight" activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -590,12 +582,12 @@
       </c>
       <c r="G1" s="13"/>
       <c r="H1" s="2" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C2" s="7">
         <v>440000</v>
@@ -609,21 +601,21 @@
       </c>
       <c r="G2" s="14"/>
       <c r="H2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C3" s="7">
         <v>440000</v>
       </c>
       <c r="D3" s="9">
-        <v>40554</v>
+        <v>39824</v>
       </c>
       <c r="E3" s="11">
         <v>0</v>
@@ -633,21 +625,21 @@
       </c>
       <c r="G3" s="14"/>
       <c r="H3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C4" s="7">
         <v>440000</v>
       </c>
       <c r="D4" s="9">
-        <v>40574</v>
+        <v>39844</v>
       </c>
       <c r="E4" s="11">
         <v>0</v>

</xml_diff>